<commit_message>
Diagram data kasus revisi 4
</commit_message>
<xml_diff>
--- a/Documents/DIAGRAM STUDI KASUS V.1.4.xlsx
+++ b/Documents/DIAGRAM STUDI KASUS V.1.4.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>RUMAH MALEBER, CIANJUR</t>
   </si>
@@ -74,12 +75,6 @@
     <t>Moda Transportasi Yg Memungkinkan :</t>
   </si>
   <si>
-    <t>Mobil(120)</t>
-  </si>
-  <si>
-    <t>Motor(100)</t>
-  </si>
-  <si>
     <t>Motor(20)</t>
   </si>
   <si>
@@ -101,15 +96,6 @@
     <t>R.M AMPERA BANDUNG</t>
   </si>
   <si>
-    <t>Mobil(20)</t>
-  </si>
-  <si>
-    <t>Motor(10)</t>
-  </si>
-  <si>
-    <t>Jalan Kaki(45)</t>
-  </si>
-  <si>
     <t>Event : Keberangkatan Menuju Stasiun</t>
   </si>
   <si>
@@ -249,13 +235,58 @@
   </si>
   <si>
     <t>Departure : 03.50 WIB</t>
+  </si>
+  <si>
+    <t>EVENT [1]</t>
+  </si>
+  <si>
+    <t>EVENT : PERTEMUAN PENGAWAS</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 19. 00 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Selesai : 21.30 WIB</t>
+  </si>
+  <si>
+    <t>PROSES</t>
+  </si>
+  <si>
+    <t>[ START ]</t>
+  </si>
+  <si>
+    <t>kereta api</t>
+  </si>
+  <si>
+    <t>Moda Transportasi  :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jl. Aceh No. 71 A, Citarum, Bandung Wetan,</t>
+  </si>
+  <si>
+    <t>RUMAH</t>
+  </si>
+  <si>
+    <t>Maleber, KarangTengah, Cianjur</t>
+  </si>
+  <si>
+    <t>Mobil(62.8Km, 125 menit)</t>
+  </si>
+  <si>
+    <t>Motor(62.2Km, 132 menit)</t>
+  </si>
+  <si>
+    <t>Jalan Kaki(58.5Km, 740 menit)</t>
+  </si>
+  <si>
+    <t>Bus(,189 menit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,8 +309,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +381,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,36 +452,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -427,13 +557,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2750344</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -480,13 +610,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2317750</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -532,15 +662,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>150601</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2360083</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>2652395</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -555,8 +685,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11410950" y="914400"/>
-          <a:ext cx="2274358" cy="0"/>
+          <a:off x="9401757" y="2214563"/>
+          <a:ext cx="2501794" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -586,13 +716,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2275417</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -639,13 +769,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2391833</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -692,13 +822,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47419</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>107156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2684140</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>107156</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -745,13 +875,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>145677</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2381250</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -798,13 +928,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>100854</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2233083</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>116416</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -851,13 +981,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>112061</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2667000</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -904,13 +1034,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>141157</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>130969</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -957,13 +1087,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2627312</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>99219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2643187</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>107156</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -981,6 +1111,64 @@
         <a:xfrm>
           <a:off x="17010062" y="1432719"/>
           <a:ext cx="15875" cy="579437"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>52107</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>84044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2507176</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>84044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B6E53E7-D448-457F-B505-EE7871D7177D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2629460" y="2840691"/>
+          <a:ext cx="2455069" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1306,407 +1494,591 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H27"/>
+  <dimension ref="B6:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="40.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="45.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="40.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="45.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="38.28515625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D6" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="F30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B9:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="D9" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="D12" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="D13" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C17" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C18" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H10" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H11" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>45</v>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="31" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="D12:D13"/>
+  <mergeCells count="1">
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>